<commit_message>
Insert data and calculation to the spread sheet are mostly done
</commit_message>
<xml_diff>
--- a/Plantilla.xlsx
+++ b/Plantilla.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos Programación\Cotizaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB6BEA2-0F3F-4565-B979-33B6F5867524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4CA4D20-79B9-4538-A2E6-364B9949F86E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Item</t>
   </si>
@@ -62,6 +75,18 @@
   </si>
   <si>
     <t>Ahorras</t>
+  </si>
+  <si>
+    <t>C. Pagina</t>
+  </si>
+  <si>
+    <t>C. Anillado</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Redondeado</t>
   </si>
 </sst>
 </file>
@@ -206,6 +231,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF27A73D"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -265,6 +295,74 @@
         </a:ln>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>25066</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>174521</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>660980</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>206387</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle: Rounded Corners 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{821C880C-5E37-486C-8A29-752F6B45F4D1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="227472" y="746021"/>
+          <a:ext cx="5832992" cy="222366"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 9944"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:srgbClr val="27A73D"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -569,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B5:M12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="148" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,9 +681,11 @@
     <col min="6" max="6" width="18" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" customWidth="1"/>
     <col min="8" max="8" width="3.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>0</v>
       </c>
@@ -604,10 +704,18 @@
       <c r="G5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
+      <c r="J5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
@@ -626,12 +734,27 @@
         <v>8</v>
       </c>
       <c r="G6" s="2">
-        <v>0</v>
+        <f>+M6</f>
+        <v>32</v>
+      </c>
+      <c r="J6">
+        <v>0.15</v>
+      </c>
+      <c r="K6">
+        <v>1.5</v>
+      </c>
+      <c r="L6">
+        <f>+D6*J6+1</f>
+        <v>32.200000000000003</v>
+      </c>
+      <c r="M6">
+        <f>+ROUND(L6,0)</f>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="2:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="6">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>9</v>
@@ -646,7 +769,22 @@
         <v>8</v>
       </c>
       <c r="G7" s="6">
-        <v>0</v>
+        <f>+M7</f>
+        <v>144</v>
+      </c>
+      <c r="J7">
+        <v>0.12</v>
+      </c>
+      <c r="K7">
+        <v>2.5</v>
+      </c>
+      <c r="L7">
+        <f>+D7*J7+1</f>
+        <v>143.79999999999998</v>
+      </c>
+      <c r="M7">
+        <f>+ROUND(L7,0)</f>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="2:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -654,7 +792,8 @@
         <v>11</v>
       </c>
       <c r="G8" s="12">
-        <v>0</v>
+        <f>+SUM(G6:G7)</f>
+        <v>176</v>
       </c>
       <c r="K8" s="4"/>
     </row>
@@ -663,7 +802,7 @@
         <v>12</v>
       </c>
       <c r="G9" s="10">
-        <v>0.08</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
@@ -671,7 +810,8 @@
         <v>13</v>
       </c>
       <c r="G10" s="11">
-        <v>0</v>
+        <f>+ROUND(G8*G9,0)</f>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="2:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -679,11 +819,20 @@
         <v>11</v>
       </c>
       <c r="G11" s="8">
-        <v>0</v>
+        <f>+G8-G10</f>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="2:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E7" xr:uid="{A5D9D9C6-A881-4D0E-88A5-113AB6A18324}">
+      <formula1>"Carta,Medio oficio,Oficio"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F7" xr:uid="{8C615919-DE72-4A39-9716-262C3A86A054}">
+      <formula1>"Blanco y negro,Colores"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Complex prie calculations added, they can be modify in excel
</commit_message>
<xml_diff>
--- a/Plantilla.xlsx
+++ b/Plantilla.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos Programación\Cotizaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4CA4D20-79B9-4538-A2E6-364B9949F86E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76690C25-6E4A-4180-B55C-7BE72AE4D132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
+    <sheet name="Precios" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>Item</t>
   </si>
@@ -87,6 +88,36 @@
   </si>
   <si>
     <t>Redondeado</t>
+  </si>
+  <si>
+    <t>Precios</t>
+  </si>
+  <si>
+    <t>Paginas</t>
+  </si>
+  <si>
+    <t>Oficio</t>
+  </si>
+  <si>
+    <t>Colores</t>
+  </si>
+  <si>
+    <t>Dificultad</t>
+  </si>
+  <si>
+    <t>Ninguna</t>
+  </si>
+  <si>
+    <t>Medio</t>
+  </si>
+  <si>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>IMPRESION</t>
+  </si>
+  <si>
+    <t>ANILLADO</t>
   </si>
 </sst>
 </file>
@@ -189,7 +220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -224,6 +255,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -323,8 +360,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="227472" y="746021"/>
-          <a:ext cx="5832992" cy="222366"/>
+          <a:off x="224891" y="754014"/>
+          <a:ext cx="5831369" cy="225030"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -667,8 +704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B5:M12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="97" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,8 +718,10 @@
     <col min="6" max="6" width="18" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" customWidth="1"/>
     <col min="8" max="8" width="3.7109375" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -704,6 +743,9 @@
       <c r="G5" s="5" t="s">
         <v>5</v>
       </c>
+      <c r="I5" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="J5" s="1" t="s">
         <v>14</v>
       </c>
@@ -725,7 +767,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="2">
-        <v>208</v>
+        <v>120</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>7</v>
@@ -735,21 +777,26 @@
       </c>
       <c r="G6" s="2">
         <f>+M6</f>
-        <v>32</v>
+        <v>21</v>
+      </c>
+      <c r="I6" t="s">
+        <v>23</v>
       </c>
       <c r="J6">
-        <v>0.15</v>
+        <f>+INDEX(Precios!C5:D7,MATCH(E6,Precios!B5:B7,0),MATCH(F6,Precios!C4:D4,0))*INDEX(Precios!C10:C12,MATCH(D6,Precios!B10:B12,1))*INDEX(Precios!C15:C17,MATCH(I6,Precios!B15:B17,0))</f>
+        <v>0.1605</v>
       </c>
       <c r="K6">
+        <f>+INDEX(Precios!G5:I16,MATCH(D6,Precios!F5:F16,1),MATCH(E6,Precios!G4:I4,0))</f>
         <v>1.5</v>
       </c>
       <c r="L6">
-        <f>+D6*J6+1</f>
-        <v>32.200000000000003</v>
+        <f>+J6*D6+K6</f>
+        <v>20.76</v>
       </c>
       <c r="M6">
         <f>+ROUND(L6,0)</f>
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="2:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -770,21 +817,7 @@
       </c>
       <c r="G7" s="6">
         <f>+M7</f>
-        <v>144</v>
-      </c>
-      <c r="J7">
-        <v>0.12</v>
-      </c>
-      <c r="K7">
-        <v>2.5</v>
-      </c>
-      <c r="L7">
-        <f>+D7*J7+1</f>
-        <v>143.79999999999998</v>
-      </c>
-      <c r="M7">
-        <f>+ROUND(L7,0)</f>
-        <v>144</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -793,9 +826,8 @@
       </c>
       <c r="G8" s="12">
         <f>+SUM(G6:G7)</f>
-        <v>176</v>
-      </c>
-      <c r="K8" s="4"/>
+        <v>21</v>
+      </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F9" s="9" t="s">
@@ -811,7 +843,7 @@
       </c>
       <c r="G10" s="11">
         <f>+ROUND(G8*G9,0)</f>
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -820,7 +852,7 @@
       </c>
       <c r="G11" s="8">
         <f>+G8-G10</f>
-        <v>164</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="2:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -834,7 +866,332 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD86AD17-81F6-4F27-8150-23E9D7AD0094}">
+  <dimension ref="B1:I17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B1" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="F1" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>0.25</v>
+      </c>
+      <c r="D5">
+        <v>0.15</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <f>+G5*1.1</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5:I16" si="0">+G5*0.75</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="D6">
+        <v>0.115</v>
+      </c>
+      <c r="F6">
+        <v>100</v>
+      </c>
+      <c r="G6">
+        <v>1.5</v>
+      </c>
+      <c r="H6">
+        <f>+G6*1.1</f>
+        <v>1.6500000000000001</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>1.125</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="D7">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="F7">
+        <v>200</v>
+      </c>
+      <c r="G7">
+        <v>1.5</v>
+      </c>
+      <c r="H7">
+        <f t="shared" ref="H7:H16" si="1">+G7*1.1</f>
+        <v>1.6500000000000001</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>1.125</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>300</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9">
+        <v>400</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>3.3000000000000003</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>1.07</v>
+      </c>
+      <c r="F10">
+        <v>500</v>
+      </c>
+      <c r="G10">
+        <v>4</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="2">
+        <v>150</v>
+      </c>
+      <c r="C11">
+        <v>1.03</v>
+      </c>
+      <c r="F11">
+        <v>600</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>5.5</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="2">
+        <v>300</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>700</v>
+      </c>
+      <c r="G12">
+        <v>6</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>6.6000000000000005</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>800</v>
+      </c>
+      <c r="G13">
+        <v>7</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>7.7000000000000011</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14">
+        <v>900</v>
+      </c>
+      <c r="G14">
+        <v>8</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1000</v>
+      </c>
+      <c r="G15">
+        <v>12</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>13.200000000000001</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16">
+        <v>1.07</v>
+      </c>
+      <c r="F16">
+        <v>2000</v>
+      </c>
+      <c r="G16">
+        <v>15</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>11.25</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17">
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="F1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>